<commit_message>
Better name parsing for prov import
</commit_message>
<xml_diff>
--- a/scripts/tests/prov-apr-2024.xlsx
+++ b/scripts/tests/prov-apr-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmaszy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9060D1CF-C929-6849-92D3-C3E8B6110178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3863966C-04FD-224E-8371-D54114A9B1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26300" windowHeight="14160" xr2:uid="{C687CB74-FCEF-444B-A73C-B3998B48CA92}"/>
   </bookViews>
@@ -705,9 +705,6 @@
     <t xml:space="preserve"> lianny@trspinalclinic.com              </t>
   </si>
   <si>
-    <t>Lianny Jimenez, Billing Specialist</t>
-  </si>
-  <si>
     <t>The Right Spinal Clinic</t>
   </si>
   <si>
@@ -1126,6 +1123,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>Lianny Jimenez</t>
   </si>
 </sst>
 </file>
@@ -1522,8 +1522,8 @@
   <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1546,10 +1546,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -2761,13 +2761,13 @@
         <v>220</v>
       </c>
       <c r="E31" t="s">
+        <v>361</v>
+      </c>
+      <c r="F31" t="s">
         <v>221</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>222</v>
-      </c>
-      <c r="G31" t="s">
-        <v>223</v>
       </c>
       <c r="H31" t="s">
         <v>48</v>
@@ -2779,7 +2779,7 @@
         <v>33614</v>
       </c>
       <c r="K31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -2791,16 +2791,16 @@
         <v>jaxinjuryc@gmail.com</v>
       </c>
       <c r="C32" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" t="s">
         <v>225</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
         <v>226</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>227</v>
-      </c>
-      <c r="G32" t="s">
-        <v>228</v>
       </c>
       <c r="H32" t="s">
         <v>35</v>
@@ -2812,7 +2812,7 @@
         <v>32223</v>
       </c>
       <c r="K32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -2824,22 +2824,22 @@
         <v>Momentum Rehab and Chiropractor</v>
       </c>
       <c r="C33" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" t="s">
         <v>230</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>231</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>232</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>233</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>234</v>
-      </c>
-      <c r="H33" t="s">
-        <v>235</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>18</v>
@@ -2848,7 +2848,7 @@
         <v>32606</v>
       </c>
       <c r="K33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
@@ -2860,19 +2860,19 @@
         <v>Journey Spinal Care</v>
       </c>
       <c r="C34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D34" t="s">
         <v>237</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>238</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>239</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>240</v>
-      </c>
-      <c r="G34" t="s">
-        <v>241</v>
       </c>
       <c r="H34" t="s">
         <v>166</v>
@@ -2884,7 +2884,7 @@
         <v>32771</v>
       </c>
       <c r="K34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
@@ -2896,19 +2896,19 @@
         <v>drcallahandc@gmail.com</v>
       </c>
       <c r="C35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" t="s">
         <v>243</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>244</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>245</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>246</v>
-      </c>
-      <c r="G35" t="s">
-        <v>247</v>
       </c>
       <c r="H35" t="s">
         <v>106</v>
@@ -2920,34 +2920,34 @@
         <v>32308</v>
       </c>
       <c r="K35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" t="e">
-        <v>#N/A</v>
+      <c r="A36">
+        <v>55</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>drcartales@gmail.com</v>
       </c>
       <c r="C36" t="s">
+        <v>248</v>
+      </c>
+      <c r="D36" t="s">
         <v>249</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>250</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>251</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>252</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>253</v>
-      </c>
-      <c r="H36" t="s">
-        <v>254</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>18</v>
@@ -2965,19 +2965,19 @@
         <v>jjscottdc@gmail.com</v>
       </c>
       <c r="C37" t="s">
+        <v>254</v>
+      </c>
+      <c r="D37" t="s">
         <v>255</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>256</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>257</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>258</v>
-      </c>
-      <c r="G37" t="s">
-        <v>259</v>
       </c>
       <c r="H37" t="s">
         <v>41</v>
@@ -2989,7 +2989,7 @@
         <v>34769</v>
       </c>
       <c r="K37" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
@@ -3001,22 +3001,22 @@
         <v>drtim@brevardchiro.com</v>
       </c>
       <c r="C38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" t="s">
         <v>261</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>262</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>263</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>264</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>265</v>
-      </c>
-      <c r="H38" t="s">
-        <v>266</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>18</v>
@@ -3034,19 +3034,19 @@
         <v>Palm Beach Physical</v>
       </c>
       <c r="C39" t="s">
+        <v>266</v>
+      </c>
+      <c r="D39" t="s">
         <v>267</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>268</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>269</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>270</v>
-      </c>
-      <c r="G39" t="s">
-        <v>271</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>18</v>
@@ -3064,22 +3064,22 @@
         <v>Legault Fam Chiropractic</v>
       </c>
       <c r="C40" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40" t="s">
         <v>272</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>273</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>274</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>275</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>276</v>
-      </c>
-      <c r="H40" t="s">
-        <v>277</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>18</v>
@@ -3097,19 +3097,19 @@
         <v>drbradleyfrick@outlook.com</v>
       </c>
       <c r="C41" t="s">
+        <v>277</v>
+      </c>
+      <c r="D41" t="s">
         <v>278</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>279</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>280</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>281</v>
-      </c>
-      <c r="G41" t="s">
-        <v>282</v>
       </c>
       <c r="H41" t="s">
         <v>199</v>
@@ -3121,16 +3121,16 @@
         <v>34110</v>
       </c>
       <c r="K41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L41" t="s">
         <v>33</v>
       </c>
       <c r="M41" t="s">
+        <v>283</v>
+      </c>
+      <c r="N41" t="s">
         <v>284</v>
-      </c>
-      <c r="N41" t="s">
-        <v>285</v>
       </c>
       <c r="O41" t="s">
         <v>18</v>
@@ -3148,22 +3148,22 @@
         <v>Chiro Express</v>
       </c>
       <c r="C42" t="s">
+        <v>285</v>
+      </c>
+      <c r="D42" t="s">
         <v>286</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>287</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
+        <v>285</v>
+      </c>
+      <c r="G42" t="s">
         <v>288</v>
       </c>
-      <c r="F42" t="s">
-        <v>286</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>289</v>
-      </c>
-      <c r="H42" t="s">
-        <v>290</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>18</v>
@@ -3172,58 +3172,58 @@
         <v>33594</v>
       </c>
       <c r="K42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
+        <v>291</v>
+      </c>
+      <c r="D46" t="s">
         <v>292</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>293</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>294</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>295</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>296</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K46" t="s">
         <v>297</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>298</v>
-      </c>
-      <c r="L46" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
+        <v>299</v>
+      </c>
+      <c r="D47" t="s">
         <v>300</v>
       </c>
-      <c r="D47" t="s">
+      <c r="I47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L47" t="s">
         <v>301</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L47" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
+        <v>302</v>
+      </c>
+      <c r="D48" t="s">
         <v>303</v>
-      </c>
-      <c r="D48" t="s">
-        <v>304</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>18</v>
@@ -3231,10 +3231,10 @@
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
+        <v>304</v>
+      </c>
+      <c r="D49" t="s">
         <v>305</v>
-      </c>
-      <c r="D49" t="s">
-        <v>306</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>18</v>
@@ -3242,30 +3242,30 @@
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
+        <v>306</v>
+      </c>
+      <c r="D50" t="s">
         <v>307</v>
       </c>
-      <c r="D50" t="s">
+      <c r="I50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L50" t="s">
         <v>308</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L50" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
+        <v>309</v>
+      </c>
+      <c r="D51" t="s">
         <v>310</v>
       </c>
-      <c r="D51" t="s">
+      <c r="I51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L51" t="s">
         <v>311</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L51" t="s">
-        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -3288,7 +3288,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3">
         <v>55</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B4">
         <v>43</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B5">
         <v>45</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B6">
         <v>26</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B7">
         <v>13039</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B8">
         <v>60</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B9">
         <v>44</v>
@@ -3352,7 +3352,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B10">
         <v>13041</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B11">
         <v>13034</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B12">
         <v>24</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B13">
         <v>61</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B14">
         <v>54</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B17">
         <v>46</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19">
         <v>57</v>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B20">
         <v>22</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B21">
         <v>18</v>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B22">
         <v>17</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B23">
         <v>23</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B24">
         <v>28</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B25">
         <v>13038</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B26">
         <v>13037</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B27">
         <v>50</v>
@@ -3496,7 +3496,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B28">
         <v>48</v>
@@ -3504,7 +3504,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B29">
         <v>56</v>
@@ -3512,7 +3512,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B30">
         <v>53</v>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B31">
         <v>25</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B33">
         <v>59</v>
@@ -3544,7 +3544,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B34">
         <v>49</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B37">
         <v>21</v>
@@ -3576,7 +3576,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B38">
         <v>13</v>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B39">
         <v>51</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B40">
         <v>27</v>
@@ -3600,7 +3600,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B41">
         <v>58</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B42">
         <v>10</v>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B43">
         <v>30</v>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B44">
         <v>15</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B45">
         <v>13036</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B46">
         <v>33</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B47">
         <v>52</v>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B48">
         <v>14</v>
@@ -3664,7 +3664,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B49">
         <v>13035</v>
@@ -3672,7 +3672,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B50">
         <v>42</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B51">
         <v>38</v>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B52">
         <v>19</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B53">
         <v>35</v>

</xml_diff>